<commit_message>
Sun May 16 00:35:13 CST 2021
</commit_message>
<xml_diff>
--- a/笔记/DOP/知识点.xlsx
+++ b/笔记/DOP/知识点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28060" windowHeight="13160"/>
+    <workbookView windowWidth="28060" windowHeight="13160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="chechlist" sheetId="2" r:id="rId1"/>
@@ -690,12 +690,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve"> 1. 上一个环节要为下一个环节考量
 2. 设计程序时要考虑易测试性、易监控性、易部署性
 3. </t>
@@ -704,7 +698,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Songti SC"/>
         <charset val="134"/>
       </rPr>
       <t>从右向左</t>
@@ -2008,12 +2002,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>1. 捣乱大猩猩: 模拟可用区域故障
 2. 捣乱金刚: 地区故障
 3. 延迟猴子: RESTful引入延迟后停机，模拟服务降级，确保相关服务正常工作
@@ -2023,7 +2011,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Songti SC"/>
         <charset val="134"/>
       </rPr>
       <t>不符合最佳实践的实例</t>
@@ -2042,7 +2030,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Songti SC"/>
         <charset val="134"/>
       </rPr>
       <t>不健康</t>
@@ -2061,7 +2049,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Songti SC"/>
         <charset val="134"/>
       </rPr>
       <t>没有混乱和浪费</t>
@@ -2079,7 +2067,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Songti SC"/>
         <charset val="134"/>
       </rPr>
       <t>搜索未使用的资源并处理</t>
@@ -2098,7 +2086,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Songti SC"/>
         <charset val="134"/>
       </rPr>
       <t>安全违规或漏洞的实例</t>
@@ -2132,19 +2120,13 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>免责事后分析会议的</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Songti SC"/>
         <charset val="134"/>
       </rPr>
       <t>第一要务</t>
@@ -2162,7 +2144,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Songti SC"/>
         <charset val="134"/>
       </rPr>
       <t>相关事件的时间线</t>
@@ -2180,7 +2162,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Songti SC"/>
         <charset val="134"/>
       </rPr>
       <t>采取的所有措施及具体时间</t>
@@ -2198,7 +2180,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Songti SC"/>
         <charset val="134"/>
       </rPr>
       <t>观察到的影响</t>
@@ -3032,6 +3014,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">职责分离: 开发人员变更提交给代码库管理员接收审查和批准变更功能，然后由IT运维将变更部署到生产环境
@@ -3538,62 +3521,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3607,9 +3536,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3623,8 +3596,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3637,10 +3611,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3652,7 +3627,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3674,6 +3649,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -3686,16 +3669,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Songti SC"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Songti SC"/>
       <charset val="134"/>
     </font>
     <font>
@@ -3706,7 +3689,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3739,25 +3722,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3775,13 +3764,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3793,7 +3776,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3805,31 +3788,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3847,37 +3812,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3895,7 +3836,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3907,25 +3896,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3991,17 +3968,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4031,21 +4008,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -4055,6 +4017,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -4093,142 +4070,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4308,6 +4285,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4315,9 +4295,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4646,7 +4623,7 @@
   <sheetPr/>
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -4662,32 +4639,32 @@
       </c>
     </row>
     <row r="2" ht="34" customHeight="1" spans="1:1">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="34" customHeight="1" spans="1:1">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" ht="32" customHeight="1" spans="1:1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" ht="32" customHeight="1" spans="1:1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="26" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" ht="32" customHeight="1" spans="1:1">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" ht="32" customHeight="1" spans="1:1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4702,7 +4679,7 @@
       </c>
     </row>
     <row r="10" ht="32" customHeight="1" spans="1:1">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4717,10 +4694,10 @@
   <sheetPr/>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="108" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="32" customHeight="1" outlineLevelCol="6"/>
@@ -4904,7 +4881,7 @@
       <c r="E10" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="23" t="s">
         <v>50</v>
       </c>
       <c r="G10" s="18"/>
@@ -4919,7 +4896,7 @@
       <c r="E11" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="24" t="s">
         <v>53</v>
       </c>
       <c r="G11" s="18"/>
@@ -5491,7 +5468,7 @@
       <c r="D48" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="E48" s="22" t="s">
+      <c r="E48" s="23" t="s">
         <v>169</v>
       </c>
       <c r="F48" s="18"/>
@@ -5507,7 +5484,7 @@
       <c r="E49" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="F49" s="19" t="s">
+      <c r="F49" s="21" t="s">
         <v>172</v>
       </c>
       <c r="G49" s="18"/>
@@ -5724,7 +5701,7 @@
   <sheetPr/>
   <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sat Jun  5 23:49:26 CST 2021
</commit_message>
<xml_diff>
--- a/笔记/DOP/知识点.xlsx
+++ b/笔记/DOP/知识点.xlsx
@@ -690,6 +690,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve"> 1. 上一个环节要为下一个环节考量
 2. 设计程序时要考虑易测试性、易监控性、易部署性
 3. </t>
@@ -907,7 +913,7 @@
     <t>DevOps角色如何增加业务价值而协作</t>
   </si>
   <si>
-    <t>1. 价值流图，识别阻碍价值流快速流动的环节，缩短前置时间和提高可靠性
+    <t>1. 价值流图，识别阻碍价值流快速流动的环节，缩短前置时间和提高可靠性。
 2. 组建专门的转型团队（拥有共同目标、保持小跨度的改进计划、为非功能性需求预留20%开发时间、减少技术债务、提高工作可视化程度）
 3. 用工作强化预期行为</t>
   </si>
@@ -2002,6 +2008,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>1. 捣乱大猩猩: 模拟可用区域故障
 2. 捣乱金刚: 地区故障
 3. 延迟猴子: RESTful引入延迟后停机，模拟服务降级，确保相关服务正常工作
@@ -2120,6 +2132,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>免责事后分析会议的</t>
     </r>
     <r>
@@ -3463,10 +3481,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -3528,6 +3546,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -3536,15 +3569,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3552,30 +3586,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3598,7 +3609,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3611,11 +3622,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3635,22 +3668,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3722,13 +3740,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3746,19 +3830,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3770,79 +3908,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3854,55 +3920,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3968,21 +3986,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -4007,6 +4010,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -4018,6 +4045,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4045,167 +4083,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4694,10 +4712,10 @@
   <sheetPr/>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="32" customHeight="1" outlineLevelCol="6"/>
@@ -5701,8 +5719,8 @@
   <sheetPr/>
   <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="2"/>

</xml_diff>